<commit_message>
id en el mapa
</commit_message>
<xml_diff>
--- a/static/Puntos.xlsx
+++ b/static/Puntos.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Barranquilla y Soledad</t>
+          <t>Bucaramanga - Floridablanca - Piedecuesta</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -478,7 +478,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0875810000000000360230</t>
+          <t>6800110000000002800616</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>10.9062691999</v>
+        <v>7.14499230679</v>
       </c>
       <c r="F2" t="n">
-        <v>-74.8091111303</v>
+        <v>-73.124413</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Barranquilla y Soledad</t>
+          <t>Bucaramanga - Floridablanca - Piedecuesta</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0875810000000000040401</t>
+          <t>6800110000000002850125</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -515,16 +515,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>10.920313452</v>
+        <v>7.15298783395</v>
       </c>
       <c r="F3" t="n">
-        <v>-74.7705287006</v>
+        <v>-73.12597473069999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Barranquilla y Soledad</t>
+          <t>Bucaramanga - Floridablanca - Piedecuesta</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0800110000000036050202</t>
+          <t>6800110000000002850513</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -543,16 +543,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>10.9351791838</v>
+        <v>7.14997382542</v>
       </c>
       <c r="F4" t="n">
-        <v>-74.7871044079</v>
+        <v>-73.1239001484</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Barranquilla y Soledad</t>
+          <t>Bucaramanga - Floridablanca - Piedecuesta</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -562,7 +562,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0800110000000017030104</t>
+          <t>6800110000000009440321</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -571,16 +571,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>10.9714742642</v>
+        <v>7.09960313404</v>
       </c>
       <c r="F5" t="n">
-        <v>-74.7970955792</v>
+        <v>-73.10988221700001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Barranquilla y Soledad</t>
+          <t>Bucaramanga - Floridablanca - Piedecuesta</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -590,7 +590,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0800110000000002020116</t>
+          <t>6827610000000000090315</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>11.022547375</v>
+        <v>7.06004692805</v>
       </c>
       <c r="F6" t="n">
-        <v>-74.8104431375</v>
+        <v>-73.0866898312</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Barranquilla y Soledad</t>
+          <t>Bucaramanga - Floridablanca - Piedecuesta</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0800110000000002020230</t>
+          <t>6827610000000000030630</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -627,16 +627,16 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>11.0232752763</v>
+        <v>7.07496927963</v>
       </c>
       <c r="F7" t="n">
-        <v>-74.8116186096</v>
+        <v>-73.0833930158</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Barranquilla y Soledad</t>
+          <t>Bucaramanga - Floridablanca - Piedecuesta</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0800110000000002060416</t>
+          <t>6800110000000012380513</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -655,16 +655,16 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>11.0167850126</v>
+        <v>7.11615102554</v>
       </c>
       <c r="F8" t="n">
-        <v>-74.8059755771</v>
+        <v>-73.1060115377</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Barranquilla y Soledad</t>
+          <t>Bucaramanga - Floridablanca - Piedecuesta</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -674,7 +674,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0800110000000011040101</t>
+          <t>6827610000000000110231</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -683,16 +683,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>10.9878831387</v>
+        <v>7.08236877722</v>
       </c>
       <c r="F9" t="n">
-        <v>-74.81927028219999</v>
+        <v>-73.109770799</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Barranquilla y Soledad</t>
+          <t>Bucaramanga - Floridablanca - Piedecuesta</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -702,7 +702,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0800110000000001020145</t>
+          <t>6800110000000010620105</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -711,10 +711,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>11.023962895</v>
+        <v>7.09316301106</v>
       </c>
       <c r="F10" t="n">
-        <v>-74.8170227983</v>
+        <v>-73.1110351889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>